<commit_message>
added discovery modules Aug-15_2025
</commit_message>
<xml_diff>
--- a/pytheas_data/modification_sets.xlsx
+++ b/pytheas_data/modification_sets.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrwill/prog/pytheas_tk_interface/pytheas_root/pytheas_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrwill/prog/Pytheas_Folder/Pytheas_Qt_root/Pytheas_Qt/pytheas_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFFEF48-C8FB-D44F-8B27-17282C69BDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECA33C4-24BE-6C4C-B066-E2C603752D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10720" yWindow="500" windowWidth="26800" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="nucleotide_table" sheetId="1" r:id="rId1"/>
+    <sheet name="modification_sets" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1714,7 +1714,7 @@
   <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>